<commit_message>
Added feature to copy and move cards
</commit_message>
<xml_diff>
--- a/.NETRequirementsTest.xlsx
+++ b/.NETRequirementsTest.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <x:si>
-    <x:t>62b61d383757c9306ea02b53</x:t>
+    <x:t>62b67a3b2be36f4542da6bcb</x:t>
   </x:si>
   <x:si>
     <x:t>Week 1</x:t>
@@ -512,7 +512,7 @@
       <x:selection activeCell="A1" sqref="A1 A1:A1"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="14.377656" defaultRowHeight="12.8" zeroHeight="false"/>
+  <x:sheetFormatPr defaultColWidth="15.798906" defaultRowHeight="12.8" zeroHeight="false"/>
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="1" t="s">

</xml_diff>